<commit_message>
added candle effect at sungnam city
</commit_message>
<xml_diff>
--- a/data/Seongnam_Sankey_2017_original.xlsx
+++ b/data/Seongnam_Sankey_2017_original.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="23715" windowHeight="9870"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="23715" windowHeight="9870" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -641,7 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -988,12 +988,12 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
   </cols>
@@ -1269,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>